<commit_message>
new build of reshow hidden marks
</commit_message>
<xml_diff>
--- a/asset/data/شهادات اعدادي جديدة.xlsx
+++ b/asset/data/شهادات اعدادي جديدة.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12000" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12000" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="نتائج 1ع" sheetId="2" r:id="rId1"/>
@@ -1984,8 +1984,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView view="pageBreakPreview" rightToLeft="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0" topLeftCell="AN75">
-      <selection activeCell="C78" sqref="A78:XFD78"/>
+    <sheetView view="pageBreakPreview" tabSelected="1" rightToLeft="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AW3" sqref="AW3:AW189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16918,8 +16918,8 @@
       <c r="AV89" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AW89" s="31">
-        <v>0</v>
+      <c r="AW89" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="AX89" s="32">
         <v>0</v>
@@ -17935,7 +17935,7 @@
         <v>10</v>
       </c>
       <c r="AW95" s="31">
-        <v>6.9000000000000004</v>
+        <v>20.899999999999999</v>
       </c>
       <c r="AX95" s="32">
         <v>19.800000000000001</v>
@@ -18177,7 +18177,7 @@
         <v>29.399999999999999</v>
       </c>
       <c r="S97" s="28">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="T97" s="30">
         <v>10</v>
@@ -18193,11 +18193,11 @@
       </c>
       <c r="X97" s="23">
         <f t="shared" si="16"/>
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="Y97" s="24">
         <f t="shared" si="17"/>
-        <v>18</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="Z97" s="28">
         <v>24</v>
@@ -18247,11 +18247,11 @@
       </c>
       <c r="AN97" s="20">
         <f t="shared" si="22"/>
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="AO97" s="24">
         <f t="shared" si="23"/>
-        <v>132.69999999999999</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="AP97" s="28">
         <v>19.600000000000001</v>
@@ -18912,24 +18912,24 @@
       <c r="AJ101" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AK101" s="30" t="s">
-        <v>56</v>
+      <c r="AK101" s="30">
+        <v>6</v>
       </c>
       <c r="AL101" s="23">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM101" s="24">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="AN101" s="20">
         <f t="shared" si="22"/>
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="AO101" s="24">
         <f t="shared" si="23"/>
-        <v>82.599999999999994</v>
+        <v>83.799999999999997</v>
       </c>
       <c r="AP101" s="28">
         <v>14</v>
@@ -20649,7 +20649,7 @@
         <v>10</v>
       </c>
       <c r="AW111" s="31">
-        <v>4.0499999999999998</v>
+        <v>21.550000000000001</v>
       </c>
       <c r="AX111" s="32">
         <v>16.600000000000001</v>
@@ -24972,27 +24972,27 @@
         <v>17.600000000000001</v>
       </c>
       <c r="Z137" s="28">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AA137" s="30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB137" s="30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC137" s="30">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AD137" s="30">
         <v>24</v>
       </c>
       <c r="AE137" s="23">
         <f t="shared" si="30"/>
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AF137" s="24">
         <f t="shared" si="31"/>
-        <v>27.600000000000001</v>
+        <v>24</v>
       </c>
       <c r="AG137" s="28">
         <v>23</v>
@@ -25019,11 +25019,11 @@
       </c>
       <c r="AN137" s="20">
         <f t="shared" si="34"/>
-        <v>441.25</v>
+        <v>429.25</v>
       </c>
       <c r="AO137" s="24">
         <f t="shared" si="35"/>
-        <v>123.39999999999999</v>
+        <v>119.8</v>
       </c>
       <c r="AP137" s="28">
         <v>17</v>
@@ -27326,18 +27326,18 @@
         <v>10</v>
       </c>
       <c r="V151" s="30">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="W151" s="30">
         <v>27</v>
       </c>
       <c r="X151" s="23">
         <f t="shared" si="28"/>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Y151" s="24">
         <f t="shared" si="29"/>
-        <v>17.800000000000001</v>
+        <v>18.199999999999999</v>
       </c>
       <c r="Z151" s="28">
         <v>28</v>
@@ -27387,11 +27387,11 @@
       </c>
       <c r="AN151" s="20">
         <f t="shared" si="34"/>
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AO151" s="24">
         <f t="shared" si="35"/>
-        <v>130.40000000000001</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="AP151" s="28">
         <v>19.800000000000001</v>
@@ -27487,7 +27487,7 @@
         <v>30</v>
       </c>
       <c r="S152" s="28">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="T152" s="30">
         <v>10</v>
@@ -27503,34 +27503,34 @@
       </c>
       <c r="X152" s="23">
         <f t="shared" si="28"/>
-        <v>86.5</v>
+        <v>96.5</v>
       </c>
       <c r="Y152" s="24">
         <f t="shared" si="29"/>
-        <v>17.300000000000001</v>
+        <v>19.300000000000001</v>
       </c>
       <c r="Z152" s="28">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AA152" s="30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AB152" s="30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AC152" s="30">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AD152" s="30">
         <v>30</v>
       </c>
       <c r="AE152" s="23">
         <f t="shared" si="30"/>
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="AF152" s="24">
         <f t="shared" si="31"/>
-        <v>24.600000000000001</v>
+        <v>30</v>
       </c>
       <c r="AG152" s="28">
         <v>30</v>
@@ -27557,11 +27557,11 @@
       </c>
       <c r="AN152" s="20">
         <f t="shared" si="34"/>
-        <v>460.5</v>
+        <v>488.5</v>
       </c>
       <c r="AO152" s="24">
         <f t="shared" si="35"/>
-        <v>129.30000000000001</v>
+        <v>136.69999999999999</v>
       </c>
       <c r="AP152" s="28">
         <v>18</v>
@@ -27995,7 +27995,7 @@
         <v>27.449999999999999</v>
       </c>
       <c r="S155" s="28">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="T155" s="30">
         <v>10</v>
@@ -28011,14 +28011,14 @@
       </c>
       <c r="X155" s="23">
         <f t="shared" si="28"/>
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="Y155" s="24">
         <f t="shared" si="29"/>
-        <v>17.199999999999999</v>
+        <v>18.199999999999999</v>
       </c>
       <c r="Z155" s="28">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="AA155" s="30">
         <v>8</v>
@@ -28034,11 +28034,11 @@
       </c>
       <c r="AE155" s="23">
         <f t="shared" si="30"/>
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AF155" s="24">
         <f t="shared" si="31"/>
-        <v>23.699999999999999</v>
+        <v>25.199999999999999</v>
       </c>
       <c r="AG155" s="28">
         <v>30</v>
@@ -28065,11 +28065,11 @@
       </c>
       <c r="AN155" s="20">
         <f t="shared" si="34"/>
-        <v>447.5</v>
+        <v>457.5</v>
       </c>
       <c r="AO155" s="24">
         <f t="shared" si="35"/>
-        <v>125.05</v>
+        <v>127.55</v>
       </c>
       <c r="AP155" s="28">
         <v>19.399999999999999</v>
@@ -28188,7 +28188,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="Z156" s="28">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AA156" s="30">
         <v>8</v>
@@ -28204,11 +28204,11 @@
       </c>
       <c r="AE156" s="23">
         <f t="shared" si="30"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AF156" s="24">
         <f t="shared" si="31"/>
-        <v>21.300000000000001</v>
+        <v>21.600000000000001</v>
       </c>
       <c r="AG156" s="28">
         <v>21</v>
@@ -28235,11 +28235,11 @@
       </c>
       <c r="AN156" s="20">
         <f t="shared" si="34"/>
-        <v>391.25</v>
+        <v>392.25</v>
       </c>
       <c r="AO156" s="24">
         <f t="shared" si="35"/>
-        <v>108.75</v>
+        <v>109.05</v>
       </c>
       <c r="AP156" s="28">
         <v>17.199999999999999</v>
@@ -30050,7 +30050,7 @@
         <v>16</v>
       </c>
       <c r="Z167" s="28">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AA167" s="30">
         <v>8</v>
@@ -30066,11 +30066,11 @@
       </c>
       <c r="AE167" s="23">
         <f t="shared" si="30"/>
-        <v>63.5</v>
+        <v>62.5</v>
       </c>
       <c r="AF167" s="24">
         <f t="shared" si="31"/>
-        <v>19.050000000000001</v>
+        <v>18.75</v>
       </c>
       <c r="AG167" s="28">
         <v>13</v>
@@ -30097,11 +30097,11 @@
       </c>
       <c r="AN167" s="20">
         <f t="shared" si="34"/>
-        <v>375.75</v>
+        <v>374.75</v>
       </c>
       <c r="AO167" s="24">
         <f t="shared" si="35"/>
-        <v>105.09999999999999</v>
+        <v>104.8</v>
       </c>
       <c r="AP167" s="28">
         <v>16.399999999999999</v>
@@ -30728,27 +30728,27 @@
         <v>15.699999999999999</v>
       </c>
       <c r="Z171" s="28">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AA171" s="30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB171" s="30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC171" s="30">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AD171" s="30">
         <v>17</v>
       </c>
       <c r="AE171" s="23">
         <f t="shared" si="30"/>
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="AF171" s="24">
         <f t="shared" si="31"/>
-        <v>25.5</v>
+        <v>20.699999999999999</v>
       </c>
       <c r="AG171" s="28">
         <v>21</v>
@@ -30775,11 +30775,11 @@
       </c>
       <c r="AN171" s="20">
         <f t="shared" si="34"/>
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="AO171" s="24">
         <f t="shared" si="35"/>
-        <v>118.85000000000001</v>
+        <v>114.05</v>
       </c>
       <c r="AP171" s="28">
         <v>16.600000000000001</v>
@@ -30896,7 +30896,7 @@
         <v>19</v>
       </c>
       <c r="Z172" s="28">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AA172" s="30">
         <v>9</v>
@@ -30912,11 +30912,11 @@
       </c>
       <c r="AE172" s="23">
         <f t="shared" si="30"/>
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AF172" s="24">
         <f t="shared" si="31"/>
-        <v>28.5</v>
+        <v>29.100000000000001</v>
       </c>
       <c r="AG172" s="28">
         <v>30</v>
@@ -30943,11 +30943,11 @@
       </c>
       <c r="AN172" s="20">
         <f t="shared" si="34"/>
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="AO172" s="24">
         <f t="shared" si="35"/>
-        <v>132.19999999999999</v>
+        <v>132.80000000000001</v>
       </c>
       <c r="AP172" s="28">
         <v>20</v>
@@ -31064,27 +31064,27 @@
         <v>10.800000000000001</v>
       </c>
       <c r="Z173" s="20">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="AA173" s="23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AB173" s="23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC173" s="23">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AD173" s="23" t="s">
         <v>56</v>
       </c>
       <c r="AE173" s="23">
         <f t="shared" si="30"/>
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="AF173" s="24">
         <f t="shared" si="31"/>
-        <v>15.6</v>
+        <v>19.800000000000001</v>
       </c>
       <c r="AG173" s="20">
         <v>22</v>
@@ -31098,24 +31098,24 @@
       <c r="AJ173" s="23">
         <v>20</v>
       </c>
-      <c r="AK173" s="23" t="s">
-        <v>56</v>
+      <c r="AK173" s="23">
+        <v>6</v>
       </c>
       <c r="AL173" s="23">
         <f t="shared" si="32"/>
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AM173" s="24">
         <f t="shared" si="33"/>
-        <v>12.4</v>
+        <v>13.6</v>
       </c>
       <c r="AN173" s="20">
         <f t="shared" si="34"/>
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="AO173" s="24">
         <f t="shared" si="35"/>
-        <v>82.400000000000006</v>
+        <v>87.800000000000011</v>
       </c>
       <c r="AP173" s="28">
         <v>16</v>
@@ -31234,7 +31234,7 @@
         <v>15.199999999999999</v>
       </c>
       <c r="Z174" s="28">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AA174" s="30">
         <v>8</v>
@@ -31250,11 +31250,11 @@
       </c>
       <c r="AE174" s="23">
         <f t="shared" si="30"/>
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF174" s="24">
         <f t="shared" si="31"/>
-        <v>19.199999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="AG174" s="28">
         <v>29</v>
@@ -31281,11 +31281,11 @@
       </c>
       <c r="AN174" s="20">
         <f t="shared" si="34"/>
-        <v>400.75</v>
+        <v>398.75</v>
       </c>
       <c r="AO174" s="24">
         <f t="shared" si="35"/>
-        <v>111.70000000000002</v>
+        <v>111.10000000000002</v>
       </c>
       <c r="AP174" s="28">
         <v>16.199999999999999</v>
@@ -31476,8 +31476,8 @@
       <c r="AV175" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AW175" s="31">
-        <v>0</v>
+      <c r="AW175" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="AX175" s="32">
         <v>0</v>
@@ -31908,7 +31908,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="Z178" s="28">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="AA178" s="30">
         <v>8</v>
@@ -31924,11 +31924,11 @@
       </c>
       <c r="AE178" s="23">
         <f t="shared" si="30"/>
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AF178" s="24">
         <f t="shared" si="31"/>
-        <v>19.199999999999999</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="AG178" s="28">
         <v>29</v>
@@ -31955,11 +31955,11 @@
       </c>
       <c r="AN178" s="20">
         <f t="shared" si="34"/>
-        <v>403.5</v>
+        <v>406.5</v>
       </c>
       <c r="AO178" s="24">
         <f t="shared" si="35"/>
-        <v>113.3</v>
+        <v>114.2</v>
       </c>
       <c r="AP178" s="28">
         <v>17.899999999999999</v>
@@ -33878,8 +33878,8 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" rightToLeft="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" topLeftCell="A67">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView rightToLeft="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" topLeftCell="AC1">
+      <selection activeCell="AZ14" sqref="AZ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38683,7 +38683,7 @@
         <v>10</v>
       </c>
       <c r="AU30" s="30">
-        <v>12.75</v>
+        <v>21.5</v>
       </c>
       <c r="AV30" s="32">
         <v>20</v>
@@ -45649,8 +45649,8 @@
       <c r="AC73" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AD73" s="30" t="s">
-        <v>56</v>
+      <c r="AD73" s="30">
+        <v>0</v>
       </c>
       <c r="AE73" s="23" t="s">
         <v>56</v>
@@ -45670,8 +45670,8 @@
       <c r="AJ73" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AK73" s="30" t="s">
-        <v>56</v>
+      <c r="AK73" s="30">
+        <v>0</v>
       </c>
       <c r="AL73" s="23" t="s">
         <v>56</v>
@@ -45685,8 +45685,8 @@
       <c r="AO73" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AP73" s="28" t="s">
-        <v>56</v>
+      <c r="AP73" s="28">
+        <v>0</v>
       </c>
       <c r="AQ73" s="30" t="s">
         <v>56</v>
@@ -45700,8 +45700,8 @@
       <c r="AT73" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AU73" s="30" t="s">
-        <v>56</v>
+      <c r="AU73" s="30">
+        <v>0</v>
       </c>
       <c r="AV73" s="32" t="s">
         <v>56</v>
@@ -46432,18 +46432,18 @@
         <v>6</v>
       </c>
       <c r="V78" s="30">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="W78" s="30">
         <v>30</v>
       </c>
       <c r="X78" s="23">
         <f t="shared" si="15"/>
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="Y78" s="24">
         <f t="shared" si="16"/>
-        <v>17.399999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="Z78" s="28">
         <v>30</v>
@@ -46493,11 +46493,11 @@
       </c>
       <c r="AN78" s="20">
         <f t="shared" si="21"/>
-        <v>474.5</v>
+        <v>480.5</v>
       </c>
       <c r="AO78" s="24">
         <f t="shared" si="21"/>
-        <v>133.65000000000001</v>
+        <v>134.85000000000002</v>
       </c>
       <c r="AP78" s="28">
         <v>19.199999999999999</v>
@@ -46594,18 +46594,18 @@
         <v>7</v>
       </c>
       <c r="V79" s="30">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="W79" s="30">
         <v>28</v>
       </c>
       <c r="X79" s="23">
         <f t="shared" si="15"/>
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="Y79" s="24">
         <f t="shared" si="16"/>
-        <v>17.399999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="Z79" s="28">
         <v>30</v>
@@ -46655,11 +46655,11 @@
       </c>
       <c r="AN79" s="20">
         <f t="shared" si="21"/>
-        <v>461.5</v>
+        <v>467.5</v>
       </c>
       <c r="AO79" s="24">
         <f t="shared" si="21"/>
-        <v>130.55000000000001</v>
+        <v>131.75</v>
       </c>
       <c r="AP79" s="28">
         <v>19.199999999999999</v>
@@ -48552,18 +48552,18 @@
         <v>7</v>
       </c>
       <c r="V91" s="23">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="W91" s="23">
         <v>29</v>
       </c>
       <c r="X91" s="23">
         <f t="shared" si="15"/>
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Y91" s="24">
         <f t="shared" si="16"/>
-        <v>18.199999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="Z91" s="20">
         <v>30</v>
@@ -48601,23 +48601,23 @@
         <v>20</v>
       </c>
       <c r="AK91" s="23">
-        <v>23.5</v>
+        <v>27.5</v>
       </c>
       <c r="AL91" s="23">
         <f t="shared" si="19"/>
-        <v>90.5</v>
+        <v>94.5</v>
       </c>
       <c r="AM91" s="24">
         <f t="shared" si="20"/>
-        <v>18.100000000000001</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AN91" s="20">
         <f t="shared" si="21"/>
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="AO91" s="24">
         <f t="shared" si="21"/>
-        <v>132.05000000000001</v>
+        <v>133.25</v>
       </c>
       <c r="AP91" s="28">
         <v>19.199999999999999</v>
@@ -51349,8 +51349,8 @@
       <c r="AC108" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AD108" s="30" t="s">
-        <v>56</v>
+      <c r="AD108" s="30">
+        <v>0</v>
       </c>
       <c r="AE108" s="23" t="s">
         <v>56</v>
@@ -51370,8 +51370,8 @@
       <c r="AJ108" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AK108" s="30" t="s">
-        <v>56</v>
+      <c r="AK108" s="30">
+        <v>0</v>
       </c>
       <c r="AL108" s="23" t="s">
         <v>56</v>
@@ -51385,8 +51385,8 @@
       <c r="AO108" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AP108" s="28" t="s">
-        <v>56</v>
+      <c r="AP108" s="28">
+        <v>0</v>
       </c>
       <c r="AQ108" s="30" t="s">
         <v>56</v>
@@ -51400,8 +51400,8 @@
       <c r="AT108" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AU108" s="30" t="s">
-        <v>56</v>
+      <c r="AU108" s="30">
+        <v>0</v>
       </c>
       <c r="AV108" s="32" t="s">
         <v>56</v>
@@ -55064,18 +55064,18 @@
         <v>7</v>
       </c>
       <c r="V131" s="23">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="W131" s="23">
         <v>30</v>
       </c>
       <c r="X131" s="23">
         <f t="shared" si="15"/>
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="Y131" s="24">
         <f t="shared" si="16"/>
-        <v>18.199999999999999</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="Z131" s="20">
         <v>30</v>
@@ -55125,11 +55125,11 @@
       </c>
       <c r="AN131" s="20">
         <f t="shared" si="21"/>
-        <v>485.5</v>
+        <v>491.5</v>
       </c>
       <c r="AO131" s="24">
         <f t="shared" si="21"/>
-        <v>136.35000000000002</v>
+        <v>137.55000000000001</v>
       </c>
       <c r="AP131" s="28">
         <v>20</v>
@@ -62835,11 +62835,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="AW1:AW2"/>
-    <mergeCell ref="AX1:AX2"/>
     <mergeCell ref="Z1:AF1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -62848,6 +62843,11 @@
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="AG1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AV1"/>
+    <mergeCell ref="AW1:AW2"/>
+    <mergeCell ref="AX1:AX2"/>
   </mergeCells>
   <pageSetup r:id="rId1" paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>